<commit_message>
Removed GPT and updated the function which saves the final data into corresponding Excel files
</commit_message>
<xml_diff>
--- a/titles_to_check.xlsx
+++ b/titles_to_check.xlsx
@@ -1,38 +1,49 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00D7E4BC"/>
+        <bgColor rgb="00D7E4BC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -40,18 +51,94 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -339,13 +426,898 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="199" customWidth="1" min="1" max="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Titles</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>A Former International Antitrust Fugitive Discusses His Experiences</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Bonner Springs man convicted of mail theft</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Arrest made following alleged indecent act in Epsom</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>A Look At A Possible Corporate Transparency Act Exemption</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Oh great, anti-vaxxer RFK Jr. officially in charge of health care now</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Father Arrested in Stara Zagora for Assaulting His Daughters, One Hospitalized</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Bulgarian Politics: Kiril Petkov Faces Trial Over Boyko Borissov's Arrest</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Woman charged in husband’s traffic death arrested in Ohio after skipped court date</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Maryland Woman Pleads Guilty to Felony Theft After Stealing $65,000 to Pay Restitution</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Cabot Lodge Securities: Regulatory Actions and Investor Concerns</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Teddi Mellencamp Being Sued by Former Employee Amid Health Battle</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Kauai police arrest suspect in critical hit-and-run</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>MHP trooper faces sexual battery charge</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Buffalo man arrested in connection to a string of burglaries during the past month</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>RAY MASSEY: Audi's new electric A6 e-tron is charged with joy</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Argentine Court Issues Warrants For Myanmar Officials Accused Of Rohingya 'Genocide'</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Former Texas, Washington WR Johntay Cook arrested for marijuana possession</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Confusing Injury-In-Fact Rules Hinder Federal Practice</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Feds allege Las Vegas man bilked investors of $24M in ponzi scheme</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>‘Without Provocation’: Florida Attorney Arrested After Allegedly Breaking Plate Over a Father’s Head at Wedding Reception Because He Allowed Family Members to Join Him In Buffer Line</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Former Texas Longhorns wide receiver arrested for second time in 10 days, records show</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>West Springfield business fined in connection with gasoline spill</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2 private surgery clinic contracts in limbo amid Alberta corruption allegations</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2/15/2025: NATIONAL: Ex-staffer busted for embezzling B10m from SSF</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2/15/2025: NATIONAL: Doctor charged with fraud</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2/15/2025: BUSINESS: Task force to probe inferior products</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Update: Arrest following indecent act, Epsom</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>$100 billion in COVID-era unemployment fraud targeted by Republicans</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>New leader takes charge of DLA Aviation activity at NAS Jacksonville</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Louisiana governor moves to extradite NY doctor (indicted by LA grand jury) who provided abortion pills to LA teen, NY governor denies the order</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>U.S. Attorney Trini Ross submits her resignation</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Former Texas wide receiver arrested for the second time in two weeks</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>St. Louis sheriff's deputy under investigation for detainee sexual assault</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Daughters of Target's Late Cofounder Raise Concern Over Company's Pullback on DEI Efforts</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>City of Seattle workers allege wage theft in proposed class action</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Daughters of Target’s late cofounder raise concern over company’s pullback on DEI efforts</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Summit County deputies arrest man suspected of hiding camera in bathroom and assist in Quandary Peak rescue</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Mahoning Co. Jail looking to house illegal immigrants arrested by ICE, Homeland Security</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Restaurant worker at Universal Orlando Citywalk files lawsuit over wage theft</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Aberdeenshire priest resigns her cure over bullying bishop</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>SLPD Chief fired for alleged misconduct</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>'Your right as a freeborn Englishman!' Tom Harwood fumes at man arrested for burning religious text</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Sandiganbayan orders arrest of ex-mayor of Negros Occidental town</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Casino Group Fails to Convince Appeals Court to Revive Lawsuit</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>REGN INVESTOR ALERT: Bronstein, Gewirtz &amp; Grossman LLC Announces that Regeneron Pharmaceuticals, Inc. Investors with Substantial Losses Have Opportunity to Lead Class Action Lawsuit</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Utah man charged with making, throwing Molotov cocktails at BYU</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Kessler Topaz Meltzer &amp;amp; Check, LLP Class Action Announcement NMRA: A Securities Fraud Class Action Lawsuit Was Filed Against Neumora Therapeutics, Inc. (NMRA)</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>ALAR INVESTOR ALERT: Robbins Geller Rudman &amp; Dowd LLP Announces that Alarum Technologies Ltd. Investors with Substantial Losses Have Opportunity to Lead the Alarum Technologies Class Action Lawsuit</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Texas judge orders New York doctor, also charged in another state, to pay fine for prescribing abortion pills</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>TGT INVESTOR ALERT: Bronstein, Gewirtz &amp;amp; Grossman LLC Announces that Target Corporation Investors with Substantial Losses Have Opportunity to Lead Class Action Lawsuit</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>EIX INVESTOR ALERT: Bronstein, Gewirtz &amp;amp; Grossman LLC Announces that Edison International Investors with Substantial Losses Have Opportunity to Lead Class Action Lawsuit</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Port Charlotte High School student arrested for possession of BB gun</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Gainey McKenna &amp; Egleston Announces A Class Action Lawsuit Has Been Filed Against FMC Corporation (FMC)</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Provisional liquidators appointed to Cork medical supplies company</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Fraud and Chargeback Trends to Watch in 2025 (Rolands Selakovs)</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>OPP Investigating Theft And Fraud</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Former Texas Longhorns, DeSoto WR arrested for second time in 10 days, records show</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>New York Doctor Blocked From Prescribing Abortion Drugs to Texans</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>NXT Investor Reminder: Kessler Topaz Meltzer &amp; Check, LLP Reminds Investors of Securities Fraud Class Action Lawsuit Filed Against Nextracker Inc. (NXT)</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>EQUITY ALERT: Rosen Law Firm Files Securities Class Action Lawsuit on Behalf of TransMedics Group, Inc. Investors – TMDX</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Tajikistan Faces Challenges in Its Pursuit of AI Dreams</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>ROSEN, A GLOBAL AND LEADING LAW FIRM, Encourages Merck &amp; Co., Inc. Investors to Secure Counsel Before Important Deadline in Securities Class Action – MRK</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Queen Anne Man Arrested Following Seattle Police, Internet Crimes Against Children Task Force Investigation</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>TGT Investors Have Opportunity to Lead Target Corporation Securities Fraud Lawsuit with the Schall Law Firm</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Daughters of Target's late cofounder raise concern over company's pullback on DEI efforts</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>'Ride or Die': Ryan Reynolds &amp; Blake Lively Receive Support from Talent Agency CEO Who Fired Justin Baldoni</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Woman Arrested For Hit-And-Run After Scraping Car On A Tree</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Olathe woman indicted for spending $260,000 on handbags with company debit card</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Man injured in fight he started, will be arrested after hospital release: Mobile police</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>CA2: Alleged inconsistencies in dog handler’s testimony didn’t necessarily make him unbelievable</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>D.Alaska: It was litigation strategy to not file a motion to suppress and cut def’s losses</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Forest Service fires 3,400 people after 'deferred resignation' deadline passes</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Developer who used dark money to attack Santa Ana City Councilman Phil Bacerra fined by the FPPC</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Permits filed for expansion at 2352 Atlantic Ave. in East New York</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Grocery Outlet Holding Corp. (GO) Investors: March 31, 2025 Filing Deadline in Securities Class Action - Contact Kessler Topaz Meltzer &amp; Check, LLP</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Oakland Port sees a new era of leadership as Kristi McKenney takes charge as executive director</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Kanye West Allegedly Paid How Much to Get His Sex Tape Scrubbed From the Internet?!</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Litigation Trend: Exempt Employees Sue for Overtime</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Toronto officer charged with aggravated assault after man seriously injured: SIU</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>St. Paul man arrested, charged after allegedly trying to sell stolen F. Scott Fitzgerald statue fragments</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Two Mass. men part of international criminal group arrested for home improvement scams, police say</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Management of Mild Traumatic Brain Injury in the Emergency Department - Trauma EXTRA Supplement (Trauma CME)</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Kessler Topaz Meltzer &amp; Check, LLP Class Action Announcement ICLR: A Securities Fraud Class Action Lawsuit Was Filed Against ICON Public Limited Company (ICLR)</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>St. Paul man arrested and charged in stolen F. Scott Fitzgerald statue, police say</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Kessler Topaz Meltzer &amp;amp; Check, LLP Class Action Announcement ICLR: A Securities Fraud Class Action Lawsuit Was Filed Against ICON Public Limited Company (ICLR)</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Released hostage Ofer Kalderon re-admitted to hospital with pneumonia</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Provisional liquidators appointed to medical firm which is allegedly owed €1.2m by HSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Another prosecutor resigns in latest fallout from Justice Department turmoil over NYC mayor's case</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>MODV Investor Alert: A Securities Fraud Class Action Lawsuit Has Been Filed Against ModivCare Inc. (MODV) - Contact Kessler Topaz Meltzer &amp;amp; Check, LLP</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>2025 Perspectives in Private Equity: AI &amp; Technology</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>Upheaval over NYC Mayor Eric Adams' case spreads as calls for his resignation grow</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Ethereum Faces $3,000 Resistance – This Utility Altcoin Just Hit 7,500% Gains in 90 Days</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Star employee quits on the spot, now ex-CEO wants to know the real reason: 'I was just given employee of the year, then 3 weeks later I put in resignation'</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>SUMOylation inhibition potentiates the glucocorticoid receptor to program growth arrest of acute lymphoblastic leukemia cells</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>Foreclosure Rate by State – January 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>Penticton police on Lakeshore Drive attempting arrest (Penticton)</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Leonard Cohen’s Estate Sues Former Trustee for Malpractice</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>Woman fined after admitting to stealing from employer</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Former Deloitte partner dinged by PCAOB for failures in Bancolombia audit</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>Toronto police officer charged with assault after man seriously injured last summer: SIU</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>NHS to conduct ‘wider review’ after children’s surgeon suspended</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>$6M Zicam false advertising class action settlement</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Minnesota agency pledges air quality monitoring improvements after Smith Foundry dispute, report says</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>Suburban Chicago Medical Device Company To Pay $1 Million To Resolve Federal Fraud Investigation</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>RIG FINAL DEADLINE: ROSEN, A HIGHLY RECOGNIZED LAW FIRM, Encourages Transocean Ltd. Investors to Secure Counsel Before Important February 24 Deadline in Securities Class Action – RIG</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>Researchers are driving the charge of zero emissions</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>SIU charges Toronto Police officer after civilian badly injured during summer arrest</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>Belleville, Quinte West area faces potential high threat from U.S. tariffs: study</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>Construction of bifunctional Se-MoSe&lt;sub&gt;2&lt;/sub&gt;-Cu&lt;sub&gt;2&lt;/sub&gt;MoS&lt;sub&gt;4&lt;/sub&gt; Z-scheme heterojunction: Its application in photoelectrochemical biosensing and photocatalytic degradation</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>Man charged with criminal damage and possessing a knife at Italian restaurant</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>Houston woman faces manslaughter charge in deadly Montrose crash</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>Kane County Sheriff: Bail Reform to Blame for Spike in Jail Population, Arrest Warrants – Aurora Beacon-News/Officer.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>FINRA Issues 2025 Annual Regulatory Oversight Report</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>Alberta new hot spot for auto theft as criminals flock to province</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>Could Pop-Up Ads Invade Your Dashboard? Stellantis Faces Backlash</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>Woman Arrested After Striking Three Vehicles (Including Two Police Cruisers) in Stolen Car</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>Imo APC spokesman resigns</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>Another prosecutor resigns in latest fallout from Justice Department turmoil over NYC mayor’s case</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>TV presenter Tim Den Besten confesses to identity theft on Grindr; case now dismissed</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>Oyomesi seek court protection from alleged arrest threat by Gov Makinde</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>13 people arrested in Croatia for illegally disposing of hazardous waste, Europol says</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>Crime Spree at CVS Stores in Northwest Results in Prison Term</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>Liverpool Coach Slot Charged With ‘Improper’ Conduct After Clash With Officials</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>Oppn calls for police action against Sawant for misleading &amp; misusing govt machinery</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>